<commit_message>
add cvs func into search_home.py
</commit_message>
<xml_diff>
--- a/Workbook.xlsx
+++ b/Workbook.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
   <si>
     <t>Address</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>pao de queijo</t>
+  </si>
+  <si>
+    <t>pao de sal</t>
   </si>
   <si>
     <t>sabonete</t>
@@ -565,7 +571,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A1056"/>
+  <dimension ref="A1:A1058"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="A2" sqref="A2"/>
@@ -639,132 +645,132 @@
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -774,161 +780,169 @@
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="60" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+    <row r="61" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="62" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="63" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="69" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1907,6 +1921,8 @@
     <row r="1054" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1055" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1056" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1057" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1058" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -2940,7 +2956,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A1061"/>
+  <dimension ref="A1:A1063"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="A2" sqref="A2"/>
@@ -2964,27 +2980,27 @@
     </row>
     <row r="3" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3009,12 +3025,12 @@
     </row>
     <row r="12" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3024,92 +3040,92 @@
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3119,12 +3135,12 @@
     </row>
     <row r="34" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3134,17 +3150,17 @@
     </row>
     <row r="37" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3154,67 +3170,67 @@
     </row>
     <row r="41" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3229,106 +3245,114 @@
     </row>
     <row r="56" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>59</v>
+      <c r="A63" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="64" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A64" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="69" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="65" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" ht="18.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="68" ht="19.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>70</v>
+      <c r="A70" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4307,6 +4331,8 @@
     <row r="1059" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1060" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1061" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1062" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1063" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -4332,37 +4358,37 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>